<commit_message>
Improved translation, small design fixes
</commit_message>
<xml_diff>
--- a/src/translation.xlsx
+++ b/src/translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_ill\Documents\GitHub\vegato-pet-shop.github.io\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B5D67E-2789-4CB5-AE08-FFC8256035F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465FB52A-43ED-4E6F-BAC9-51D002E46870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{292DDA69-629D-4828-9D77-5CE4949AA0A9}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>ENG</t>
   </si>
@@ -67,12 +67,6 @@
     <t>shop now</t>
   </si>
   <si>
-    <t>Products</t>
-  </si>
-  <si>
-    <t>Tooted</t>
-  </si>
-  <si>
     <t>DRY FOOD FOR CATS</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>главная</t>
   </si>
   <si>
-    <t>Продукты</t>
-  </si>
-  <si>
     <t>Сухая еда для котов</t>
   </si>
   <si>
@@ -248,6 +239,24 @@
   </si>
   <si>
     <t>Plant-based pet&lt;br&gt;food for optimal&lt;br&gt;health</t>
+  </si>
+  <si>
+    <t>in cart</t>
+  </si>
+  <si>
+    <t>ostukorvis</t>
+  </si>
+  <si>
+    <t>в корзине</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>продукты</t>
+  </si>
+  <si>
+    <t>tooted</t>
   </si>
 </sst>
 </file>
@@ -608,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971A19D9-4586-4F47-8D23-E44EBCDB03EC}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -635,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -643,13 +652,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -657,219 +666,230 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added russian translation for notice
</commit_message>
<xml_diff>
--- a/src/translation.xlsx
+++ b/src/translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_ill\Documents\GitHub\vegato-pet-shop.github.io\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465FB52A-43ED-4E6F-BAC9-51D002E46870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23545520-9F7B-41B4-AF42-7FA9FEB1E3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{292DDA69-629D-4828-9D77-5CE4949AA0A9}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>ENG</t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>tooted</t>
+  </si>
+  <si>
+    <t>Мы все еще находимся в процессе приобретения товара, но вы можете сделать предварительный заказ, чтобы мы знали, что вы заинтересованы. Мы свяжемся с вами, когда товар будет в наличии, чтобы договориться об оплате.</t>
+  </si>
+  <si>
+    <t>We are still in the process of acquiring stock, but you are welcome to pre-order so we know that you are interested. We are going to contact you when stock is available to arrange payment.</t>
   </si>
 </sst>
 </file>
@@ -617,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971A19D9-4586-4F47-8D23-E44EBCDB03EC}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -890,6 +896,17 @@
       </c>
       <c r="C24" s="1" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added why and feed pages
</commit_message>
<xml_diff>
--- a/src/translation.xlsx
+++ b/src/translation.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_ill\Documents\GitHub\vegato-pet-shop.github.io\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B56E02E-B9FF-4513-878D-4F512E211476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F732FC02-D68E-4266-BA47-8B0E2D850BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1766" windowWidth="16080" windowHeight="13603" xr2:uid="{292DDA69-629D-4828-9D77-5CE4949AA0A9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{292DDA69-629D-4828-9D77-5CE4949AA0A9}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">translation!$B$1:$D$24</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">translation!$B$1:$D$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="182">
   <si>
     <t>ENG</t>
   </si>
@@ -314,6 +314,285 @@
   </si>
   <si>
     <t>Klõpsake allalaadimiseks</t>
+  </si>
+  <si>
+    <t>Veterinary formula:</t>
+  </si>
+  <si>
+    <t>Ingredients: Corn protein, rice, corn, sunflower oil, peas, dehydrated potato, tapioca, rice bran, yeast, rice protein, wheat protein, vegetable hydrolysate (vegetarian palate), apple pulp, calcium carbonate, barley, algae oil, algae, dehydrated vegetables (pumpkin, alfalfa, carrot, plum, cranberry, parsley, sage, thyme, liquorice, canine rose, spirulina, oregano, mint, yucca schidigera (reduces the odor of pet stools), chicory (rich in FOS)), chloride, sodium chloride, monocalcium phosphate, plant extracts (citrus, grape peel, green tea, dandelion, aloe vera).</t>
+  </si>
+  <si>
+    <t>Formula developed by specialised veterinarians based on FEDIAF guidelines.</t>
+  </si>
+  <si>
+    <t>Complete food, no supplementation necessary.</t>
+  </si>
+  <si>
+    <t>Contains optimal amounts of Taurine, Vitamin A, Vitamin B12 and Arachidonic Acid: Substances considered essential for cats, in addition to L-methionine, L-tryptophan and L-lysine.</t>
+  </si>
+  <si>
+    <t>Improves cats' lives:</t>
+  </si>
+  <si>
+    <t>Contains methionine and cranberries to protect the urinary system from infections and crystals.</t>
+  </si>
+  <si>
+    <t>Contains antioxidant tocopherols.</t>
+  </si>
+  <si>
+    <t>Contains pumpkin, with healthy fibre to help regulate digestion.</t>
+  </si>
+  <si>
+    <t>Contains tapioca, which strengthens bones and contains a lot of iron.</t>
+  </si>
+  <si>
+    <t>Low-fat: suitable for neutered, overweight and obese animals.</t>
+  </si>
+  <si>
+    <t>Veterinaarvalem</t>
+  </si>
+  <si>
+    <t>Koostis: Maisiproteiin, riis, mais, päevalilleõli, herned, dehüdreeritud kartul, tapiokk, riisikliid, pärm, riisiproteiin, nisuproteiin, taimne hüdrolüsaat (taimetoit), õuna viljaliha, kaltsiumkarbonaat, oder, vetikaõli, vetikad, kuivatatud köögiviljad (kõrvits, lutsern, porgand, ploom, jõhvikas, petersell, salvei, tüümian, lagrits, koerroos, spirulina, pune, piparmünt, yucca schidigera (vähendab lemmikloomade väljaheidete lõhna), sigur (rikas FOS allikas)), kloriid, naatriumkloriid, monokaltsiumfosfaat, taimeekstraktid ( tsitruselised, viinamarjakoor, roheline tee, võilill, aloe vera).</t>
+  </si>
+  <si>
+    <t>Loomaarstide poolt välja töötatud valem, mis põhineb FEDIAF juhistel.</t>
+  </si>
+  <si>
+    <t>Täisväärtuslik toit, toidulisandeid pole vaja.</t>
+  </si>
+  <si>
+    <t>Sisaldab optimaalses koguses tauriini, A-vitamiini, B12-vitamiini ja arahhidoonhapet: lisaks L-metioniinile, L-trüptofaanile ja L-lüsiinile on kassidele olulised ained.</t>
+  </si>
+  <si>
+    <t>Kasside elu parandamine:</t>
+  </si>
+  <si>
+    <t>Sisaldab metioniini ja jõhvikaid, et kaitsta kuseteede süsteemi infektsioonide ja kristallide eest.</t>
+  </si>
+  <si>
+    <t>Sisaldab antioksüdantseid tokoferoole.</t>
+  </si>
+  <si>
+    <t>Sisaldab sigurit, rikas FOS allikas. Sisaldab L-trüptofaani ja L-lüsiini.</t>
+  </si>
+  <si>
+    <t>Sisaldab kõrvitsat, tervislikke kiudaineid, mis aitavad reguleerida seedimist.</t>
+  </si>
+  <si>
+    <t>Sisaldab tapiokki, mis tugevdab luid ja sisaldab palju rauda.</t>
+  </si>
+  <si>
+    <t>Madala rasvasisaldusega: sobib steriliseeritud, ülekaalulistele ja rasvunud loomadele.</t>
+  </si>
+  <si>
+    <t>Ветеринарная формула</t>
+  </si>
+  <si>
+    <t>Состав: Кукурузный белок, рис, кукуруза, подсолнечное масло, горох, обезвоженный картофель, тапиока, рисовые отруби, дрожжи, рисовый белок, пшеничный белок, растительный гидролизат (вегетарианский вкус), яблочная мякоть, карбонат кальция, ячмень, масло водорослей, водоросли, обезвоженные овощи (тыква, люцерна, морковь, слива, клюква, петрушка, шалфей, тимьян, лакрица, собачья роза, спирулина, орегано, мята, юкка Шидигера (уменьшает запах экскрементов питомца), цикорий (богатый источник ФОС)), хлорид, хлорид натрия, монокальцийфосфат, растительные экстракты ( цитрусовые, кожура винограда, зеленый чай, одуванчик, алоэ вера).</t>
+  </si>
+  <si>
+    <t>Формула разработана ветеринарами на основе рекомендаций европейской федерации производителей кормов для домашних животных (FEDIAF).</t>
+  </si>
+  <si>
+    <t>Полноценное питание, никаких добавок не требуется.</t>
+  </si>
+  <si>
+    <t>Содержит оптимальное количество таурина, витамина А, витамина В12 и арахидоновой кислоты: веществ, считающихся незаменимыми для кошек, в дополнение к L-метионину, L-триптофану и L-лизину.</t>
+  </si>
+  <si>
+    <t>Улучшает жизни кошек:</t>
+  </si>
+  <si>
+    <t>Содержит метионин и клюкву для защиты мочевыделительной системы от инфекций и кристаллов.</t>
+  </si>
+  <si>
+    <t>Содержит антиоксидантные токоферолы.</t>
+  </si>
+  <si>
+    <t>Содержит цикорий, богатый ФОС.</t>
+  </si>
+  <si>
+    <t>Содержит L-триптофан и L-лизин.</t>
+  </si>
+  <si>
+    <t>Содержит тыкву со здоровой клетчаткой, которая помогает регулировать пищеварение.</t>
+  </si>
+  <si>
+    <t>Contains chicory, rich in FOS.</t>
+  </si>
+  <si>
+    <t>Contains L-tryptophan and L-lysine.</t>
+  </si>
+  <si>
+    <t>Sisaldab L-trüptofaani ja L-lüsiini.</t>
+  </si>
+  <si>
+    <t>Содержит тапиоку, которая укрепляет кости и содержит много железа.</t>
+  </si>
+  <si>
+    <t>С низким содержанием жира: подходит для кастрированных животных, животных с избыточным весом и ожирением.</t>
+  </si>
+  <si>
+    <t>Uses:</t>
+  </si>
+  <si>
+    <t>Healthy cats, or cats that do not have specific nutritional needs.</t>
+  </si>
+  <si>
+    <t>Obese cats that need to lose weight.</t>
+  </si>
+  <si>
+    <t>Cats allergic or intolerant to animal products.</t>
+  </si>
+  <si>
+    <t>Cats with skin problems.</t>
+  </si>
+  <si>
+    <t>Cats with arthrosis.</t>
+  </si>
+  <si>
+    <t>Cats with immune-compromised conditions.</t>
+  </si>
+  <si>
+    <t>Neutered cats.</t>
+  </si>
+  <si>
+    <t>Cats that have had crystalluria.</t>
+  </si>
+  <si>
+    <t>Pregnant and lactating cats.</t>
+  </si>
+  <si>
+    <t>For all breeds and sizes.</t>
+  </si>
+  <si>
+    <t>Kasutusjuhtumid:</t>
+  </si>
+  <si>
+    <t>Terved kassid või kassid, kellel ei ole spetsiifilisi toitumisvajadusi.</t>
+  </si>
+  <si>
+    <t>Rasvunud kassid, kes peavad kaalust alla võtma.</t>
+  </si>
+  <si>
+    <t>Kassid loomsete saaduste suhtes allergilised või talumatud.</t>
+  </si>
+  <si>
+    <t>Nahaprobleemidega kassid.</t>
+  </si>
+  <si>
+    <t>Artroosiga kassid.</t>
+  </si>
+  <si>
+    <t>Kassid, kellel on nõrgenenud immuunsus.</t>
+  </si>
+  <si>
+    <t>Kastreeritud kassid.</t>
+  </si>
+  <si>
+    <t>Kassid, kellel on olnud kristalluuria.</t>
+  </si>
+  <si>
+    <t>Rasedad ja imetavad kassid.</t>
+  </si>
+  <si>
+    <t>Kõigile tõugudele ja suurustele.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Подходит для: </t>
+  </si>
+  <si>
+    <t>Здоровые кошки или кошки, у которых нет особых потребностей в питании.</t>
+  </si>
+  <si>
+    <t>Тучные кошки, которым необходимо похудеть.</t>
+  </si>
+  <si>
+    <t>Кошки с аллергией или непереносимостью продуктов животного происхождения.</t>
+  </si>
+  <si>
+    <t>Кошки с проблемами кожи.</t>
+  </si>
+  <si>
+    <t>Кошки с артрозом.</t>
+  </si>
+  <si>
+    <t>Кошки с ослабленным иммунитетом.</t>
+  </si>
+  <si>
+    <t>Стерилизованные кошки.</t>
+  </si>
+  <si>
+    <t>Кошки, у которых была кристаллурия.</t>
+  </si>
+  <si>
+    <t>Беременные и кормящие кошки.</t>
+  </si>
+  <si>
+    <t>Для всех пород и размеров.</t>
+  </si>
+  <si>
+    <t>100% plant-based and natural:</t>
+  </si>
+  <si>
+    <t>Free from addictive substances, medicines, toxins and hormones contained in meat products.</t>
+  </si>
+  <si>
+    <t>Free from chemical flavourings, it contains natural flavouring: with substances extracted directly from nature, without the harmful health consequences of chemical flavourings.</t>
+  </si>
+  <si>
+    <t>Vitamins, provitamins, trace elements and minerals per kg:</t>
+  </si>
+  <si>
+    <t>Technological additives: Tocopherol extracts from vegetable oils.</t>
+  </si>
+  <si>
+    <t>Analytical Components:</t>
+  </si>
+  <si>
+    <t>Crude Protein 28%</t>
+  </si>
+  <si>
+    <t>Fats 12%</t>
+  </si>
+  <si>
+    <t>Crude Fibre 3%</t>
+  </si>
+  <si>
+    <t>Organic Matter or Ashes 6%</t>
+  </si>
+  <si>
+    <t>Calcium 0.8%</t>
+  </si>
+  <si>
+    <t>Phosphorus 0.75%</t>
+  </si>
+  <si>
+    <t>EPA + DHA 0.09%</t>
+  </si>
+  <si>
+    <t>Arachidonic acid 0.06%</t>
+  </si>
+  <si>
+    <t>Metabolizable Energy 3690kcal/kg</t>
+  </si>
+  <si>
+    <t>FEED</t>
+  </si>
+  <si>
+    <t>КОРМ</t>
+  </si>
+  <si>
+    <t>TOIT</t>
+  </si>
+  <si>
+    <t>WHY</t>
+  </si>
+  <si>
+    <t>ПОЧЕМУ</t>
+  </si>
+  <si>
+    <t>MIKS</t>
   </si>
 </sst>
 </file>
@@ -675,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971A19D9-4586-4F47-8D23-E44EBCDB03EC}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -731,6 +1010,9 @@
       </c>
     </row>
     <row r="4" spans="1:4">
+      <c r="A4" t="b">
+        <v>1</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
@@ -742,287 +1024,287 @@
       </c>
     </row>
     <row r="5" spans="1:4">
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>176</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4">
+      <c r="A6" t="b">
+        <v>1</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>180</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>56</v>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="B16" t="s">
+    <row r="18" spans="1:4">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="B17" t="s">
+    <row r="19" spans="1:4">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="B23" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="b">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="b">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="b">
         <v>1</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>88</v>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1030,13 +1312,497 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="b">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="b">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="b">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="b">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="b">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="b">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="b">
+        <v>1</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="b">
+        <v>1</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="b">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="b">
+        <v>1</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="b">
+        <v>1</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="b">
+        <v>1</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="b">
+        <v>1</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="b">
+        <v>1</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="b">
+        <v>1</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="b">
+        <v>1</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="b">
+        <v>1</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="b">
+        <v>1</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="b">
+        <v>1</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="b">
+        <v>1</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="b">
+        <v>1</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="b">
+        <v>1</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="b">
+        <v>1</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added text for translation
</commit_message>
<xml_diff>
--- a/src/translation.xlsx
+++ b/src/translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_ill\Documents\GitHub\vegato-pet-shop.github.io\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8B884E-FF07-4EB9-9A41-31FE3F8E95D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928890F5-236B-40AF-BFFB-FC36F93BC570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{292DDA69-629D-4828-9D77-5CE4949AA0A9}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
   <si>
     <t>ENG</t>
   </si>
@@ -596,6 +596,27 @@
   </si>
   <si>
     <t>safety</t>
+  </si>
+  <si>
+    <t>Conventional meat-based pet food uses ingredients not suited for human consumption. This means that there are much less regulations in place which results in &lt;b&gt;wide-spread contamination&lt;/b&gt; with toxic compounds such as:</t>
+  </si>
+  <si>
+    <t>An ongoing and increasing contamination with toxic elements. &lt;b&gt;Heavy metals&lt;/b&gt; including arsenic, cadmium, nickel, lead, antimony, &lt;b&gt;radioactive elements&lt;/b&gt; such as uranium and thorium and other elements such as beryllium routinely go way above safe limits. [1,2]</t>
+  </si>
+  <si>
+    <t>Endocrine disrupting compounds such as PCBs and PBDEs. [5]</t>
+  </si>
+  <si>
+    <t>Nitrate and nitrite used in meat processing are routinely &lt;b&gt;two to three times the safety limit&lt;/b&gt;. [2] Chronic exposure can result in cardiac and thyroid diseases as well as cancer. [4]</t>
+  </si>
+  <si>
+    <t>Mycotoxin contamination&lt;/b&gt; above safe limits of all products irrespective of marketing channels. The long-term exposure to mycotoxins is implicated in numerous clinical conditions such as vomiting, reduced immunity and cancer. [3]</t>
+  </si>
+  <si>
+    <t>VeggieAnimals plant-based pet food is formulated from human grade ingredients which ensures that your pet is kept as healthy as possible and does not suffer needlessly from contaminants.</t>
+  </si>
+  <si>
+    <t>References:</t>
   </si>
 </sst>
 </file>
@@ -957,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971A19D9-4586-4F47-8D23-E44EBCDB03EC}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1733,6 +1754,41 @@
     <row r="72" spans="2:2">
       <c r="B72" s="3" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added translation and changed font
</commit_message>
<xml_diff>
--- a/src/translation.xlsx
+++ b/src/translation.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daria\Documents\GitHub\vegato-pet-shop.github.io\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_ill\Documents\GitHub\vegato-pet-shop.github.io\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3E2681-BDC9-4CD9-BA8C-3A169D90438A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF765E7-EDA6-47DE-97A2-769F75B236DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="21599" windowHeight="11872" xr2:uid="{292DDA69-629D-4828-9D77-5CE4949AA0A9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{292DDA69-629D-4828-9D77-5CE4949AA0A9}"/>
   </bookViews>
   <sheets>
     <sheet name="translation" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">translation!$B$1:$D$26</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">translation!$B$1:$D$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="280">
   <si>
     <t>ENG</t>
   </si>
@@ -394,12 +394,6 @@
     <t>Полноценное питание, никаких добавок не требуется.</t>
   </si>
   <si>
-    <t>Содержит оптимальное количество таурина, витамина А, витамина В12 и арахидоновой кислоты: веществ, считающихся незаменимыми для кошек, в дополнение к L-метионину, L-триптофану и L-лизину.</t>
-  </si>
-  <si>
-    <t>Улучшает жизни кошек:</t>
-  </si>
-  <si>
     <t>Содержит метионин и клюкву для защиты мочевыделительной системы от инфекций и кристаллов.</t>
   </si>
   <si>
@@ -499,30 +493,6 @@
     <t xml:space="preserve">Подходит для: </t>
   </si>
   <si>
-    <t>Здоровые кошки или кошки, у которых нет особых потребностей в питании.</t>
-  </si>
-  <si>
-    <t>Тучные кошки, которым необходимо похудеть.</t>
-  </si>
-  <si>
-    <t>Кошки с аллергией или непереносимостью продуктов животного происхождения.</t>
-  </si>
-  <si>
-    <t>Кошки с проблемами кожи.</t>
-  </si>
-  <si>
-    <t>Кошки с артрозом.</t>
-  </si>
-  <si>
-    <t>Кошки с ослабленным иммунитетом.</t>
-  </si>
-  <si>
-    <t>Стерилизованные кошки.</t>
-  </si>
-  <si>
-    <t>Кошки, у которых была кристаллурия.</t>
-  </si>
-  <si>
     <t>Беременные и кормящие кошки.</t>
   </si>
   <si>
@@ -547,33 +517,6 @@
     <t>Analytical Components:</t>
   </si>
   <si>
-    <t>Crude Protein 28%</t>
-  </si>
-  <si>
-    <t>Fats 12%</t>
-  </si>
-  <si>
-    <t>Crude Fibre 3%</t>
-  </si>
-  <si>
-    <t>Organic Matter or Ashes 6%</t>
-  </si>
-  <si>
-    <t>Calcium 0.8%</t>
-  </si>
-  <si>
-    <t>Phosphorus 0.75%</t>
-  </si>
-  <si>
-    <t>EPA + DHA 0.09%</t>
-  </si>
-  <si>
-    <t>Arachidonic acid 0.06%</t>
-  </si>
-  <si>
-    <t>Metabolizable Energy 3690kcal/kg</t>
-  </si>
-  <si>
     <t>FEED</t>
   </si>
   <si>
@@ -655,60 +598,6 @@
     <t>Аналитические компоненты:</t>
   </si>
   <si>
-    <t>Сырой белок 28%</t>
-  </si>
-  <si>
-    <t>toorvalk 28%</t>
-  </si>
-  <si>
-    <t>rasvad 12%</t>
-  </si>
-  <si>
-    <t>Жиры 12%</t>
-  </si>
-  <si>
-    <t>Toorkiud 3%</t>
-  </si>
-  <si>
-    <t>Сырая клетчатка 3%</t>
-  </si>
-  <si>
-    <t>Органические вещества или зола 6%</t>
-  </si>
-  <si>
-    <t>Orgaaniline aine või tuhk 6%</t>
-  </si>
-  <si>
-    <t>Kaltsium 0,8%</t>
-  </si>
-  <si>
-    <t>Кальций 0,8%</t>
-  </si>
-  <si>
-    <t>Фосфор 0,75%</t>
-  </si>
-  <si>
-    <t>Fosfor 0,75%</t>
-  </si>
-  <si>
-    <t>EPA + DHA 0,09%</t>
-  </si>
-  <si>
-    <t>ЭПК + ДГК 0,09%</t>
-  </si>
-  <si>
-    <t>Арахидоновая кислота 0,06%</t>
-  </si>
-  <si>
-    <t>Arahhidoonhape 0,06%</t>
-  </si>
-  <si>
-    <t>Metaboliseeritav energia 3690kcal/kg</t>
-  </si>
-  <si>
-    <t>Метаболизируемая энергия 3690 ккал/кг</t>
-  </si>
-  <si>
     <t>почему на растительной основе?</t>
   </si>
   <si>
@@ -755,6 +644,249 @@
   </si>
   <si>
     <t>Kasutatud allikad:</t>
+  </si>
+  <si>
+    <t>CATS</t>
+  </si>
+  <si>
+    <t>DOGS</t>
+  </si>
+  <si>
+    <t>КОТЫ</t>
+  </si>
+  <si>
+    <t>СОБАКИ</t>
+  </si>
+  <si>
+    <t>KASSID</t>
+  </si>
+  <si>
+    <t>KOERAD</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Nutritional information</t>
+  </si>
+  <si>
+    <t>Uses</t>
+  </si>
+  <si>
+    <t>Ингредиенты</t>
+  </si>
+  <si>
+    <t>Koostisained</t>
+  </si>
+  <si>
+    <t>Тучные коты, которым необходимо похудеть.</t>
+  </si>
+  <si>
+    <t>Коты с аллергией или непереносимостью продуктов животного происхождения.</t>
+  </si>
+  <si>
+    <t>Коты с проблемами кожи.</t>
+  </si>
+  <si>
+    <t>Коты с артрозом.</t>
+  </si>
+  <si>
+    <t>Коты с ослабленным иммунитетом.</t>
+  </si>
+  <si>
+    <t>Коты, у которых была кристаллурия.</t>
+  </si>
+  <si>
+    <t>Показания</t>
+  </si>
+  <si>
+    <t>Toiteväärtus</t>
+  </si>
+  <si>
+    <t>Пищевая ценность</t>
+  </si>
+  <si>
+    <t>Содержит оптимальное количество таурина, витамина А, витамина В12 и арахидоновой кислоты: веществ, считающихся незаменимыми для котов, в дополнение к L-метионину, L-триптофану и L-лизину.</t>
+  </si>
+  <si>
+    <t>Улучшает жизни котов:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> мг</t>
+  </si>
+  <si>
+    <t>Kasutusjuhtumid</t>
+  </si>
+  <si>
+    <t>Improves dogs' lives:</t>
+  </si>
+  <si>
+    <t>Koerte elu parandamine:</t>
+  </si>
+  <si>
+    <t>Улучшает жизни собак:</t>
+  </si>
+  <si>
+    <t>Фосфор</t>
+  </si>
+  <si>
+    <t>Кальций</t>
+  </si>
+  <si>
+    <t>Органические вещества или зола</t>
+  </si>
+  <si>
+    <t>Сырая клетчатка</t>
+  </si>
+  <si>
+    <t>Жиры</t>
+  </si>
+  <si>
+    <t>Сырой белок</t>
+  </si>
+  <si>
+    <t>ЭПК + ДГК</t>
+  </si>
+  <si>
+    <t>Арахидоновая кислота</t>
+  </si>
+  <si>
+    <t>kcal/kg</t>
+  </si>
+  <si>
+    <t>Metabolizable Energy</t>
+  </si>
+  <si>
+    <t>ккал/кг</t>
+  </si>
+  <si>
+    <t>Метаболизируемая энергия</t>
+  </si>
+  <si>
+    <t>Metaboliseeritav energia</t>
+  </si>
+  <si>
+    <t>Arahhidoonhape</t>
+  </si>
+  <si>
+    <t>EPA + DHA</t>
+  </si>
+  <si>
+    <t>Fosfor</t>
+  </si>
+  <si>
+    <t>Kaltsium</t>
+  </si>
+  <si>
+    <t>Orgaaniline aine või tuhk</t>
+  </si>
+  <si>
+    <t>Toorkiud</t>
+  </si>
+  <si>
+    <t>Toorvalk</t>
+  </si>
+  <si>
+    <t>Rasvad</t>
+  </si>
+  <si>
+    <t>Healthy dogs, or dogs that do not have specific nutritional needs.</t>
+  </si>
+  <si>
+    <t>Dogs with allergies or intolerances to animal products.</t>
+  </si>
+  <si>
+    <t>Dogs with atopy, if they are not allergic to any of our ingredients.</t>
+  </si>
+  <si>
+    <t>Dogs with arthrosis.</t>
+  </si>
+  <si>
+    <t>Dogs with autoimmune conditions.</t>
+  </si>
+  <si>
+    <t>Neutered dogs.</t>
+  </si>
+  <si>
+    <t>Dogs with skin problems.</t>
+  </si>
+  <si>
+    <t>Dogs with digestive problems.</t>
+  </si>
+  <si>
+    <t>Suitable for overweight or obese dogs.</t>
+  </si>
+  <si>
+    <t>Suitable for all breeds and sizes.</t>
+  </si>
+  <si>
+    <t>Беременные и кормящие собаки.</t>
+  </si>
+  <si>
+    <t>Собаки, у которых была кристаллурия.</t>
+  </si>
+  <si>
+    <t>Стерилизованные собаки.</t>
+  </si>
+  <si>
+    <t>Кастрированные коты.</t>
+  </si>
+  <si>
+    <t>Собаки с ослабленным иммунитетом.</t>
+  </si>
+  <si>
+    <t>Собаки с артрозом.</t>
+  </si>
+  <si>
+    <t>Собаки с проблемами кожи.</t>
+  </si>
+  <si>
+    <t>Собаки с аллергией или непереносимостью продуктов животного происхождения.</t>
+  </si>
+  <si>
+    <t>Тучные собаки, которым необходимо похудеть.</t>
+  </si>
+  <si>
+    <t>Здоровые собаки, у которых нет особых потребностей в питании.</t>
+  </si>
+  <si>
+    <t>Здоровые коты, у которых нет особых потребностей в питании.</t>
+  </si>
+  <si>
+    <t>Terved kassid, kellel ei ole spetsiifilisi toitumisvajadusi.</t>
+  </si>
+  <si>
+    <t>Ingredients: Corn protein, rice, corn, sunflower oil, peas, dehydrated potato, tapioca, rice bran, yeast, rice protein, wheat protein, hydrolysed vegetables (vegetarian palatant), apple pulp, calcium carbonate, barley, seaweed oil, seaweed, dehydrated vegetables (pumpkin, alfalfa, carrot, plum, blueberry, parsley, sage, thyme, liquorice, honeysuckle, spirulina, oregano, mint, yucca Schidigera, chicory (rich in FOS)), potassium chloride, sodium chloride, monocalcium phosphate, plant extracts (citrus, grape peel, green tea, dandelion, aloe vera)</t>
+  </si>
+  <si>
+    <t>Состав: кукурузный белок, рис, кукуруза, подсолнечное масло, горох, обезвоженный картофель, тапиока, рисовые отруби, дрожжи, рисовый белок, пшеничный белок, растительный гидролизат, яблочная мякоть, карбонат кальция, ячмень, масло водорослей, водоросли, обезвоженные овощи (тыква, люцерна, морковь, слива, клюква, петрушка, шалфей, тимьян, лакрица, собачья роза, спирулина, орегано, мята, юкка Шидигера (уменьшает запах экскрементов питомца), цикорий (богатый источник ФОС)), хлорид, хлорид натрия, монокальцийфосфат, растительные экстракты ( цитрусовые, кожура винограда, зеленый чай, одуванчик, алоэ вера).</t>
+  </si>
+  <si>
+    <t>Koostis: maisiproteiin, riis, mais, päevalilleõli, herned, dehüdreeritud kartul, tapiokk, riisikliid, pärm, riisiproteiin, nisuproteiin, taimne hüdrolüsaat, õuna viljaliha, kaltsiumkarbonaat, oder, vetikaõli, vetikad, kuivatatud köögiviljad (kõrvits, lutsern, porgand, ploom, jõhvikas, petersell, salvei, tüümian, lagrits, koerroos, spirulina, pune, piparmünt, yucca schidigera (vähendab lemmikloomade väljaheidete lõhna), sigur (rikas FOS allikas)), kloriid, naatriumkloriid, monokaltsiumfosfaat, taimeekstraktid ( tsitruselised, viinamarjakoor, roheline tee, võilill, aloe vera).</t>
+  </si>
+  <si>
+    <t>Crude Fibre</t>
+  </si>
+  <si>
+    <t>Organic Matter or Ashes</t>
+  </si>
+  <si>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>Phosphorus</t>
+  </si>
+  <si>
+    <t>Arachidonic acid</t>
+  </si>
+  <si>
+    <t>Fats</t>
+  </si>
+  <si>
+    <t>Crude Protein</t>
   </si>
 </sst>
 </file>
@@ -1117,22 +1249,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971A19D9-4586-4F47-8D23-E44EBCDB03EC}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" customWidth="1"/>
+    <col min="1" max="1" width="9.3828125" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="38.46484375" customWidth="1"/>
+    <col min="3" max="3" width="38.4609375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1179,52 +1311,46 @@
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="b">
-        <v>1</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>199</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="b">
-        <v>1</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1232,13 +1358,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1246,13 +1372,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1260,13 +1386,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1274,27 +1400,27 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="b">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1302,27 +1428,27 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>56</v>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1330,13 +1456,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1344,69 +1470,69 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="b">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
-        <v>34</v>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="b">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
-        <v>37</v>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>45</v>
+      <c r="B20" t="s">
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>8</v>
+      <c r="B21" t="s">
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1414,13 +1540,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1428,13 +1554,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1442,13 +1568,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1456,13 +1582,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1470,13 +1596,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1484,13 +1610,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1498,573 +1624,788 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="B29" s="1" t="s">
+    <row r="31" spans="1:4">
+      <c r="B31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="B30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="B31" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="B32" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="1" t="s">
-        <v>88</v>
+      <c r="B33" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>117</v>
+        <v>219</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>118</v>
+        <v>220</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" t="s">
-        <v>123</v>
+      <c r="B42" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="B44" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C44" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="1" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="1" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>152</v>
+        <v>268</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>141</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>156</v>
+        <v>213</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>157</v>
+        <v>214</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="B55" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>158</v>
+        <v>261</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="B56" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>159</v>
+        <v>215</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="1" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>191</v>
+        <v>148</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="B58" s="1" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D58" t="s">
-        <v>192</v>
+        <v>149</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" s="1" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D59" t="s">
-        <v>195</v>
+        <v>171</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="D60" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="B61" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C61" t="s">
-        <v>199</v>
+        <v>152</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="D61" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="B62" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C62" t="s">
-        <v>201</v>
+        <v>153</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="D62" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="B63" s="1" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C63" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="D63" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="1" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C64" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="D64" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="2:4">
-      <c r="B65" s="1" t="s">
-        <v>168</v>
+      <c r="B65" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="C65" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="D65" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="2:4">
-      <c r="B66" s="1" t="s">
-        <v>169</v>
+      <c r="B66" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="C66" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="D66" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="2:4">
-      <c r="B67" s="1" t="s">
-        <v>170</v>
+      <c r="B67" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="C67" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="D67" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C68" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D68" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="B69" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="D69" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="B70" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C70" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="D70" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="B71" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C71" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D71" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="B72" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C72" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="D72" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
     </row>
     <row r="73" spans="2:4">
       <c r="B73" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C73" t="s">
+        <v>224</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4">
+      <c r="B74" t="s">
+        <v>248</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="B75" t="s">
+        <v>249</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" t="s">
+        <v>250</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" t="s">
+        <v>251</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" t="s">
+        <v>252</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" t="s">
+        <v>253</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="B80" t="s">
+        <v>254</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="B81" t="s">
+        <v>255</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" t="s">
+        <v>256</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83" t="s">
+        <v>257</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" t="s">
+        <v>270</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C85" t="s">
+        <v>208</v>
+      </c>
+      <c r="D85" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C86" t="s">
+        <v>218</v>
+      </c>
+      <c r="D86" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C87" t="s">
+        <v>216</v>
+      </c>
+      <c r="D87" t="s">
         <v>223</v>
       </c>
-      <c r="D73" t="s">
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C88" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="74" spans="2:4">
-      <c r="B74" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="D88" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C89" t="s">
+        <v>232</v>
+      </c>
+      <c r="D89" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C90" t="s">
+        <v>231</v>
+      </c>
+      <c r="D90" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="B91" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C91" t="s">
+        <v>230</v>
+      </c>
+      <c r="D91" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C92" t="s">
+        <v>229</v>
+      </c>
+      <c r="D92" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C93" t="s">
         <v>228</v>
       </c>
-      <c r="D74" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4">
-      <c r="B75" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C75" t="s">
-        <v>229</v>
-      </c>
-      <c r="D75" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4">
-      <c r="B76" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="D93" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C94" t="s">
         <v>227</v>
       </c>
-      <c r="D76" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4">
-      <c r="B77" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C77" t="s">
-        <v>230</v>
-      </c>
-      <c r="D77" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4">
-      <c r="B78" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C78" t="s">
-        <v>232</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="D94" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="B95" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C95" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="79" spans="2:4">
-      <c r="B79" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="D95" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C96" t="s">
         <v>234</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D96" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C97" t="s">
+        <v>238</v>
+      </c>
+      <c r="D97" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" t="s">
+        <v>235</v>
+      </c>
+      <c r="C98" t="s">
+        <v>237</v>
+      </c>
+      <c r="D98" t="s">
         <v>235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added discount and itella
</commit_message>
<xml_diff>
--- a/src/translation.xlsx
+++ b/src/translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_ill\Documents\GitHub\vegato-pet-shop.github.io\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550C8FD0-E9C3-4271-AA49-4B8DBE244BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE4ECC5-3B67-4829-BA8F-7961772B8656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="translation" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">translation!$B$1:$D$28</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">translation!$B$1:$D$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="297">
   <si>
     <t>safety</t>
   </si>
@@ -157,24 +157,6 @@
     <t xml:space="preserve">кг </t>
   </si>
   <si>
-    <t>DPD parcel locker (3 EUR)</t>
-  </si>
-  <si>
-    <t>DPD почтомат (3 EUR)</t>
-  </si>
-  <si>
-    <t>DPD pakiautomaat (3 EUR)</t>
-  </si>
-  <si>
-    <t>Omniva parcel locker (3.50 EUR)</t>
-  </si>
-  <si>
-    <t>Omniva почтомат (3.50 EUR)</t>
-  </si>
-  <si>
-    <t>Omniva pakiautomaat (3.50 EUR)</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -914,6 +896,24 @@
   </si>
   <si>
     <t>Kiri</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>proovimiseks</t>
+  </si>
+  <si>
+    <t>пробник</t>
+  </si>
+  <si>
+    <t>parcel locker</t>
+  </si>
+  <si>
+    <t>почтомат</t>
+  </si>
+  <si>
+    <t>pakiautomaat</t>
   </si>
 </sst>
 </file>
@@ -1283,8 +1283,8 @@
   </sheetPr>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1419,13 +1419,13 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C11" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D11" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="19.5" customHeight="1">
@@ -1436,7 +1436,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D12" t="s">
         <v>33</v>
@@ -1450,7 +1450,7 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -1503,13 +1503,13 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C17" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D17" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19.5" customHeight="1">
@@ -1517,13 +1517,13 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C18" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D18" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="19.5" customHeight="1">
@@ -1531,27 +1531,24 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C19" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D19" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="19.5" customHeight="1">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>294</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>295</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="19.5" customHeight="1">
@@ -1559,13 +1556,13 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>258</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>263</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="19.5" customHeight="1">
@@ -1573,13 +1570,13 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>264</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>269</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>265</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="19.5" customHeight="1">
@@ -1587,13 +1584,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="19.5" customHeight="1">
@@ -1601,13 +1598,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="19.5" customHeight="1">
@@ -1615,13 +1612,13 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="19.5" customHeight="1">
@@ -1629,13 +1626,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="19.5" customHeight="1">
@@ -1643,13 +1640,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="19.5" customHeight="1">
@@ -1657,13 +1654,13 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="19.5" customHeight="1">
@@ -1671,13 +1668,13 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="19.5" customHeight="1">
@@ -1685,819 +1682,816 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>288</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>289</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="19.5" customHeight="1">
-      <c r="A31" t="s">
-        <v>25</v>
-      </c>
       <c r="B31" t="s">
-        <v>294</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>295</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>296</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="19.5" customHeight="1">
       <c r="B32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="19.5" customHeight="1">
       <c r="B33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="19.5" customHeight="1">
       <c r="B34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="19.5" customHeight="1">
       <c r="B35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="19.5" customHeight="1">
       <c r="B36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="19.5" customHeight="1">
       <c r="B37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="19.5" customHeight="1">
       <c r="B38" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="19.5" customHeight="1">
       <c r="B39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="19.5" customHeight="1">
       <c r="B40" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="19.5" customHeight="1">
       <c r="B41" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="19.5" customHeight="1">
       <c r="B42" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="19.5" customHeight="1">
       <c r="B43" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="19.5" customHeight="1">
       <c r="B44" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="19.5" customHeight="1">
       <c r="B45" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="19.5" customHeight="1">
       <c r="B46" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D46" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="19.5" customHeight="1">
       <c r="B47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D47" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="19.5" customHeight="1">
       <c r="B48" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D48" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="19.5" customHeight="1">
       <c r="B49" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="19.5" customHeight="1">
       <c r="B50" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="19.5" customHeight="1">
       <c r="B51" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C51" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D51" t="s">
-        <v>132</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="19.5" customHeight="1">
       <c r="B52" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D52" t="s">
-        <v>263</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="19.5" customHeight="1">
       <c r="B53" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="19.5" customHeight="1">
       <c r="B54" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="19.5" customHeight="1">
       <c r="B55" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C55" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D55" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="19.5" customHeight="1">
       <c r="B56" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D56" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="19.5" customHeight="1">
       <c r="B57" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D57" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="19.5" customHeight="1">
       <c r="B58" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="19.5" customHeight="1">
       <c r="B59" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
-      </c>
-      <c r="D59" t="s">
-        <v>156</v>
+        <v>152</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="19.5" customHeight="1">
       <c r="B60" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C60" t="s">
-        <v>158</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="D60" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="2:4" ht="19.5" customHeight="1">
       <c r="B61" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C61" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D61" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="19.5" customHeight="1">
       <c r="B62" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C62" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D62" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="2:4" ht="19.5" customHeight="1">
       <c r="B63" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C63" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D63" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="2:4" ht="19.5" customHeight="1">
       <c r="B64" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C64" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D64" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="2:4" ht="19.5" customHeight="1">
       <c r="B65" t="s">
-        <v>172</v>
+        <v>267</v>
       </c>
       <c r="C65" t="s">
-        <v>173</v>
+        <v>268</v>
       </c>
       <c r="D65" t="s">
-        <v>174</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" spans="2:4" ht="19.5" customHeight="1">
       <c r="B66" t="s">
-        <v>273</v>
+        <v>169</v>
       </c>
       <c r="C66" t="s">
-        <v>274</v>
+        <v>170</v>
       </c>
       <c r="D66" t="s">
-        <v>275</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="2:4" ht="19.5" customHeight="1">
       <c r="B67" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C67" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D67" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="2:4" ht="19.5" customHeight="1">
       <c r="B68" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C68" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D68" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="2:4" ht="19.5" customHeight="1">
       <c r="B69" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C69" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D69" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="2:4" ht="19.5" customHeight="1">
       <c r="B70" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C70" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D70" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="2:4" ht="19.5" customHeight="1">
       <c r="B71" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C71" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D71" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="19.5" customHeight="1">
       <c r="B72" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C72" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D72" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="2:4" ht="19.5" customHeight="1">
       <c r="B73" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C73" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D73" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="2:4" ht="19.5" customHeight="1">
       <c r="B74" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C74" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D74" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="2:4" ht="19.5" customHeight="1">
       <c r="B75" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C75" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D75" t="s">
-        <v>201</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="2:4" ht="19.5" customHeight="1">
       <c r="B76" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C76" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D76" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="2:4" ht="19.5" customHeight="1">
       <c r="B77" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C77" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D77" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="2:4" ht="19.5" customHeight="1">
       <c r="B78" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C78" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D78" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="2:4" ht="19.5" customHeight="1">
       <c r="B79" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C79" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D79" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="2:4" ht="19.5" customHeight="1">
       <c r="B80" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C80" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D80" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="2:4" ht="19.5" customHeight="1">
       <c r="B81" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C81" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D81" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="2:4" ht="19.5" customHeight="1">
       <c r="B82" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C82" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D82" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="2:4" ht="19.5" customHeight="1">
       <c r="B83" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C83" t="s">
-        <v>217</v>
+        <v>149</v>
       </c>
       <c r="D83" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="2:4" ht="19.5" customHeight="1">
       <c r="B84" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C84" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
       <c r="D84" t="s">
-        <v>156</v>
+        <v>215</v>
       </c>
     </row>
     <row r="85" spans="2:4" ht="19.5" customHeight="1">
       <c r="B85" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C85" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D85" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="2:4" ht="19.5" customHeight="1">
       <c r="B86" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C86" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D86" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="87" spans="2:4" ht="19.5" customHeight="1">
       <c r="B87" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C87" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D87" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="88" spans="2:4" ht="19.5" customHeight="1">
       <c r="B88" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C88" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D88" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="89" spans="2:4" ht="19.5" customHeight="1">
       <c r="B89" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C89" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D89" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90" spans="2:4" ht="19.5" customHeight="1">
       <c r="B90" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C90" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D90" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="91" spans="2:4" ht="19.5" customHeight="1">
       <c r="B91" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C91" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D91" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" spans="2:4" ht="19.5" customHeight="1">
       <c r="B92" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C92" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D92" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="2:4" ht="19.5" customHeight="1">
       <c r="B93" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C93" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D93" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="94" spans="2:4" ht="19.5" customHeight="1">
       <c r="B94" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C94" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D94" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="95" spans="2:4" ht="19.5" customHeight="1">
       <c r="B95" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C95" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D95" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="2:4" ht="19.5" customHeight="1">
       <c r="B96" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C96" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D96" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="97" spans="2:4" ht="19.5" customHeight="1">
       <c r="B97" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C97" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D97" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="19.5" customHeight="1">
       <c r="B98" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C98" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D98" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" ht="19.5" customHeight="1">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
       <c r="B99" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="C99" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="D99" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
     </row>
     <row r="100" spans="2:4">
       <c r="B100" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C100" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D100" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="B101" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C101" t="s">
+        <v>282</v>
+      </c>
+      <c r="D101" t="s">
         <v>281</v>
-      </c>
-      <c r="D101" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="102" spans="2:4">
       <c r="B102" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C102" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D102" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" spans="2:4">
       <c r="B103" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C103" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D103" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added transportation support for other countries
</commit_message>
<xml_diff>
--- a/src/translation.xlsx
+++ b/src/translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_ill\Documents\GitHub\vegato-pet-shop.github.io\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE4ECC5-3B67-4829-BA8F-7961772B8656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00A3DE1-85BF-4F2C-94C8-8C4753A8DA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="312">
   <si>
     <t>safety</t>
   </si>
@@ -914,6 +914,51 @@
   </si>
   <si>
     <t>pakiautomaat</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Эстония</t>
+  </si>
+  <si>
+    <t>Латвия</t>
+  </si>
+  <si>
+    <t>Литва</t>
+  </si>
+  <si>
+    <t>Финляндия</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Finalnd</t>
+  </si>
+  <si>
+    <t>Eesti</t>
+  </si>
+  <si>
+    <t>Läti</t>
+  </si>
+  <si>
+    <t>Leedu</t>
+  </si>
+  <si>
+    <t>Soome</t>
+  </si>
+  <si>
+    <t>Country:</t>
+  </si>
+  <si>
+    <t>Riik:</t>
+  </si>
+  <si>
+    <t>Страна:</t>
   </si>
 </sst>
 </file>
@@ -1281,10 +1326,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -2417,7 +2462,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="97" spans="2:4" ht="19.5" customHeight="1">
+    <row r="97" spans="1:4" ht="19.5" customHeight="1">
       <c r="B97" t="s">
         <v>250</v>
       </c>
@@ -2428,7 +2473,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="98" spans="2:4" ht="19.5" customHeight="1">
+    <row r="98" spans="1:4" ht="19.5" customHeight="1">
       <c r="B98" t="s">
         <v>253</v>
       </c>
@@ -2439,7 +2484,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="99" spans="2:4">
+    <row r="99" spans="1:4">
       <c r="B99" t="s">
         <v>270</v>
       </c>
@@ -2450,7 +2495,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="100" spans="2:4">
+    <row r="100" spans="1:4">
       <c r="B100" t="s">
         <v>271</v>
       </c>
@@ -2461,7 +2506,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="101" spans="2:4">
+    <row r="101" spans="1:4">
       <c r="B101" t="s">
         <v>279</v>
       </c>
@@ -2472,7 +2517,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="102" spans="2:4">
+    <row r="102" spans="1:4">
       <c r="B102" t="s">
         <v>283</v>
       </c>
@@ -2483,7 +2528,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="103" spans="2:4">
+    <row r="103" spans="1:4">
       <c r="B103" t="s">
         <v>291</v>
       </c>
@@ -2492,6 +2537,73 @@
       </c>
       <c r="D103" t="s">
         <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="b">
+        <v>1</v>
+      </c>
+      <c r="B104" t="s">
+        <v>297</v>
+      </c>
+      <c r="C104" t="s">
+        <v>298</v>
+      </c>
+      <c r="D104" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="b">
+        <v>1</v>
+      </c>
+      <c r="B105" t="s">
+        <v>302</v>
+      </c>
+      <c r="C105" t="s">
+        <v>299</v>
+      </c>
+      <c r="D105" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="b">
+        <v>1</v>
+      </c>
+      <c r="B106" t="s">
+        <v>303</v>
+      </c>
+      <c r="C106" t="s">
+        <v>300</v>
+      </c>
+      <c r="D106" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="b">
+        <v>1</v>
+      </c>
+      <c r="B107" t="s">
+        <v>304</v>
+      </c>
+      <c r="C107" t="s">
+        <v>301</v>
+      </c>
+      <c r="D107" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="B108" t="s">
+        <v>309</v>
+      </c>
+      <c r="C108" t="s">
+        <v>311</v>
+      </c>
+      <c r="D108" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>